<commit_message>
added missing notz to pdf
</commit_message>
<xml_diff>
--- a/databyset.xlsx
+++ b/databyset.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\Projects\arkhamdividers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1B934BA8-BF84-40F2-BFBD-B5DDBD1ADEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3680CD31-13F1-477B-B47E-662F17E1677D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="databyset" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2528" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2540" uniqueCount="679">
   <si>
     <t>set</t>
   </si>
@@ -2090,7 +2090,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2924,13 +2924,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D319"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90:F92"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="69" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7404,12 +7410,12 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7616,13 +7622,55 @@
         <v>115</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" t="s">
+        <v>195</v>
+      </c>
+      <c r="D15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C17" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -7753,7 +7801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -8011,7 +8059,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -8241,7 +8289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -8499,7 +8547,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -8611,7 +8659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -8827,7 +8875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -8916,7 +8964,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -9244,7 +9292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -9558,7 +9606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -9606,7 +9654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -9892,7 +9940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:D23"/>
   <sheetViews>
@@ -10234,7 +10282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -10520,7 +10568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr codeName="Sheet24"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -10595,7 +10643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -10895,7 +10943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr codeName="Sheet26"/>
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -11293,7 +11341,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr codeName="Sheet27"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -11382,7 +11430,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -11429,7 +11477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -11490,7 +11538,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -11860,7 +11908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -11978,11 +12026,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="G1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12082,7 +12130,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -12157,7 +12205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:D7"/>
   <sheetViews>

</xml_diff>